<commit_message>
discover implemented, compare finished
</commit_message>
<xml_diff>
--- a/data/Soort.xlsx
+++ b/data/Soort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Daniël\Documents\UvA - AI\Jaar 3\Scriptie\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC5C3B7-CC33-4EE7-AA6B-6A9E576A9895}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D7C6F-C8B1-4922-B29A-AD631A717B8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="794">
   <si>
     <t>ID</t>
   </si>
@@ -2075,9 +2075,6 @@
   </si>
   <si>
     <t>Halammohydra vermiformis</t>
-  </si>
-  <si>
-    <t>179</t>
   </si>
   <si>
     <t>Halcampa chrysanthellum</t>
@@ -2785,8 +2782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
+      <selection activeCell="B321" sqref="B321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,38 +7145,47 @@
       <c r="A319">
         <v>402</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B319">
+        <v>179</v>
+      </c>
+      <c r="D319" t="s">
         <v>684</v>
-      </c>
-      <c r="D319" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>403</v>
       </c>
+      <c r="B320">
+        <v>270</v>
+      </c>
       <c r="D320" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>404</v>
       </c>
+      <c r="B321">
+        <v>270</v>
+      </c>
       <c r="C321" t="s">
+        <v>686</v>
+      </c>
+      <c r="D321" t="s">
         <v>687</v>
-      </c>
-      <c r="D321" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>405</v>
       </c>
+      <c r="B322">
+        <v>270</v>
+      </c>
       <c r="D322" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -7190,10 +7196,10 @@
         <v>609</v>
       </c>
       <c r="C323" t="s">
+        <v>689</v>
+      </c>
+      <c r="D323" t="s">
         <v>690</v>
-      </c>
-      <c r="D323" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -7204,7 +7210,7 @@
         <v>647</v>
       </c>
       <c r="D324" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -7212,10 +7218,10 @@
         <v>411</v>
       </c>
       <c r="B325" t="s">
+        <v>692</v>
+      </c>
+      <c r="D325" t="s">
         <v>693</v>
-      </c>
-      <c r="D325" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -7223,13 +7229,13 @@
         <v>412</v>
       </c>
       <c r="B326" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C326" t="s">
+        <v>694</v>
+      </c>
+      <c r="D326" t="s">
         <v>695</v>
-      </c>
-      <c r="D326" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -7237,10 +7243,10 @@
         <v>413</v>
       </c>
       <c r="B327" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D327" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -7248,13 +7254,13 @@
         <v>414</v>
       </c>
       <c r="B328" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C328" t="s">
+        <v>697</v>
+      </c>
+      <c r="D328" t="s">
         <v>698</v>
-      </c>
-      <c r="D328" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -7262,10 +7268,10 @@
         <v>415</v>
       </c>
       <c r="B329" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D329" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -7276,10 +7282,10 @@
         <v>606</v>
       </c>
       <c r="C330" t="s">
+        <v>700</v>
+      </c>
+      <c r="D330" t="s">
         <v>701</v>
-      </c>
-      <c r="D330" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -7290,10 +7296,10 @@
         <v>535</v>
       </c>
       <c r="C331" t="s">
+        <v>702</v>
+      </c>
+      <c r="D331" t="s">
         <v>703</v>
-      </c>
-      <c r="D331" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -7301,13 +7307,13 @@
         <v>418</v>
       </c>
       <c r="B332" t="s">
+        <v>704</v>
+      </c>
+      <c r="C332" t="s">
         <v>705</v>
       </c>
-      <c r="C332" t="s">
+      <c r="D332" t="s">
         <v>706</v>
-      </c>
-      <c r="D332" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -7315,10 +7321,10 @@
         <v>419</v>
       </c>
       <c r="B333" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D333" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -7329,7 +7335,7 @@
         <v>672</v>
       </c>
       <c r="D334" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -7340,7 +7346,7 @@
         <v>591</v>
       </c>
       <c r="D335" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -7351,7 +7357,7 @@
         <v>591</v>
       </c>
       <c r="D336" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -7362,7 +7368,7 @@
         <v>609</v>
       </c>
       <c r="D337" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -7373,7 +7379,7 @@
         <v>609</v>
       </c>
       <c r="D338" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -7384,10 +7390,10 @@
         <v>609</v>
       </c>
       <c r="C339" t="s">
+        <v>713</v>
+      </c>
+      <c r="D339" t="s">
         <v>714</v>
-      </c>
-      <c r="D339" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -7398,7 +7404,7 @@
         <v>609</v>
       </c>
       <c r="D340" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -7409,7 +7415,7 @@
         <v>563</v>
       </c>
       <c r="D341" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -7417,10 +7423,10 @@
         <v>428</v>
       </c>
       <c r="B342" t="s">
+        <v>717</v>
+      </c>
+      <c r="D342" t="s">
         <v>718</v>
-      </c>
-      <c r="D342" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -7431,7 +7437,7 @@
         <v>657</v>
       </c>
       <c r="D343" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -7442,7 +7448,7 @@
         <v>630</v>
       </c>
       <c r="D344" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,10 +7456,10 @@
         <v>431</v>
       </c>
       <c r="B345" t="s">
+        <v>721</v>
+      </c>
+      <c r="D345" t="s">
         <v>722</v>
-      </c>
-      <c r="D345" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -7461,10 +7467,10 @@
         <v>432</v>
       </c>
       <c r="B346" t="s">
+        <v>723</v>
+      </c>
+      <c r="D346" t="s">
         <v>724</v>
-      </c>
-      <c r="D346" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -7472,13 +7478,13 @@
         <v>433</v>
       </c>
       <c r="B347" t="s">
+        <v>725</v>
+      </c>
+      <c r="C347" t="s">
         <v>726</v>
       </c>
-      <c r="C347" t="s">
+      <c r="D347" t="s">
         <v>727</v>
-      </c>
-      <c r="D347" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.25">
@@ -7489,7 +7495,7 @@
         <v>627</v>
       </c>
       <c r="D348" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7500,10 +7506,10 @@
         <v>582</v>
       </c>
       <c r="C349" t="s">
+        <v>729</v>
+      </c>
+      <c r="D349" t="s">
         <v>730</v>
-      </c>
-      <c r="D349" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -7511,10 +7517,10 @@
         <v>436</v>
       </c>
       <c r="B350" t="s">
+        <v>731</v>
+      </c>
+      <c r="D350" t="s">
         <v>732</v>
-      </c>
-      <c r="D350" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -7522,13 +7528,13 @@
         <v>437</v>
       </c>
       <c r="B351" t="s">
+        <v>733</v>
+      </c>
+      <c r="C351" t="s">
         <v>734</v>
       </c>
-      <c r="C351" t="s">
+      <c r="D351" t="s">
         <v>735</v>
-      </c>
-      <c r="D351" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7536,13 +7542,13 @@
         <v>438</v>
       </c>
       <c r="B352" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C352" t="s">
+        <v>736</v>
+      </c>
+      <c r="D352" t="s">
         <v>737</v>
-      </c>
-      <c r="D352" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -7553,10 +7559,10 @@
         <v>580</v>
       </c>
       <c r="C353" t="s">
+        <v>738</v>
+      </c>
+      <c r="D353" t="s">
         <v>739</v>
-      </c>
-      <c r="D353" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -7567,10 +7573,10 @@
         <v>609</v>
       </c>
       <c r="C354" t="s">
+        <v>740</v>
+      </c>
+      <c r="D354" t="s">
         <v>741</v>
-      </c>
-      <c r="D354" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -7581,10 +7587,10 @@
         <v>609</v>
       </c>
       <c r="C355" t="s">
+        <v>742</v>
+      </c>
+      <c r="D355" t="s">
         <v>743</v>
-      </c>
-      <c r="D355" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -7595,10 +7601,10 @@
         <v>609</v>
       </c>
       <c r="C356" t="s">
+        <v>744</v>
+      </c>
+      <c r="D356" t="s">
         <v>745</v>
-      </c>
-      <c r="D356" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -7609,10 +7615,10 @@
         <v>609</v>
       </c>
       <c r="C357" t="s">
+        <v>746</v>
+      </c>
+      <c r="D357" t="s">
         <v>747</v>
-      </c>
-      <c r="D357" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -7623,7 +7629,7 @@
         <v>591</v>
       </c>
       <c r="D358" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7634,7 +7640,7 @@
         <v>609</v>
       </c>
       <c r="D359" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -7642,13 +7648,13 @@
         <v>446</v>
       </c>
       <c r="B360" t="s">
+        <v>750</v>
+      </c>
+      <c r="C360" t="s">
         <v>751</v>
       </c>
-      <c r="C360" t="s">
+      <c r="D360" t="s">
         <v>752</v>
-      </c>
-      <c r="D360" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -7659,10 +7665,10 @@
         <v>603</v>
       </c>
       <c r="C361" t="s">
+        <v>753</v>
+      </c>
+      <c r="D361" t="s">
         <v>754</v>
-      </c>
-      <c r="D361" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -7670,13 +7676,13 @@
         <v>449</v>
       </c>
       <c r="B362" t="s">
+        <v>755</v>
+      </c>
+      <c r="C362" t="s">
         <v>756</v>
       </c>
-      <c r="C362" t="s">
+      <c r="D362" t="s">
         <v>757</v>
-      </c>
-      <c r="D362" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -7684,13 +7690,13 @@
         <v>457</v>
       </c>
       <c r="B363" t="s">
+        <v>758</v>
+      </c>
+      <c r="C363" t="s">
         <v>759</v>
       </c>
-      <c r="C363" t="s">
+      <c r="D363" t="s">
         <v>760</v>
-      </c>
-      <c r="D363" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -7701,10 +7707,10 @@
         <v>545</v>
       </c>
       <c r="C364" t="s">
+        <v>761</v>
+      </c>
+      <c r="D364" t="s">
         <v>762</v>
-      </c>
-      <c r="D364" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7715,10 +7721,10 @@
         <v>545</v>
       </c>
       <c r="C365" t="s">
+        <v>763</v>
+      </c>
+      <c r="D365" t="s">
         <v>764</v>
-      </c>
-      <c r="D365" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7729,10 +7735,10 @@
         <v>545</v>
       </c>
       <c r="C366" t="s">
+        <v>765</v>
+      </c>
+      <c r="D366" t="s">
         <v>766</v>
-      </c>
-      <c r="D366" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -7743,10 +7749,10 @@
         <v>545</v>
       </c>
       <c r="C367" t="s">
+        <v>767</v>
+      </c>
+      <c r="D367" t="s">
         <v>768</v>
-      </c>
-      <c r="D367" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7757,7 +7763,7 @@
         <v>613</v>
       </c>
       <c r="D368" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7768,10 +7774,10 @@
         <v>613</v>
       </c>
       <c r="C369" t="s">
+        <v>770</v>
+      </c>
+      <c r="D369" t="s">
         <v>771</v>
-      </c>
-      <c r="D369" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7779,13 +7785,13 @@
         <v>464</v>
       </c>
       <c r="B370" t="s">
+        <v>772</v>
+      </c>
+      <c r="C370" t="s">
         <v>773</v>
       </c>
-      <c r="C370" t="s">
+      <c r="D370" t="s">
         <v>774</v>
-      </c>
-      <c r="D370" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
@@ -7793,13 +7799,13 @@
         <v>465</v>
       </c>
       <c r="B371" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C371" t="s">
+        <v>775</v>
+      </c>
+      <c r="D371" t="s">
         <v>776</v>
-      </c>
-      <c r="D371" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7810,7 +7816,7 @@
         <v>535</v>
       </c>
       <c r="D372" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7821,10 +7827,10 @@
         <v>535</v>
       </c>
       <c r="C373" t="s">
+        <v>778</v>
+      </c>
+      <c r="D373" t="s">
         <v>779</v>
-      </c>
-      <c r="D373" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -7832,10 +7838,10 @@
         <v>468</v>
       </c>
       <c r="B374" t="s">
+        <v>780</v>
+      </c>
+      <c r="D374" t="s">
         <v>781</v>
-      </c>
-      <c r="D374" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7846,7 +7852,7 @@
         <v>613</v>
       </c>
       <c r="D375" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -7857,7 +7863,7 @@
         <v>613</v>
       </c>
       <c r="D376" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7868,7 +7874,7 @@
         <v>535</v>
       </c>
       <c r="D377" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
@@ -7879,7 +7885,7 @@
         <v>535</v>
       </c>
       <c r="D378" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7890,10 +7896,10 @@
         <v>647</v>
       </c>
       <c r="C379" t="s">
+        <v>786</v>
+      </c>
+      <c r="D379" t="s">
         <v>787</v>
-      </c>
-      <c r="D379" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
@@ -7904,10 +7910,10 @@
         <v>538</v>
       </c>
       <c r="C380" t="s">
+        <v>788</v>
+      </c>
+      <c r="D380" t="s">
         <v>789</v>
-      </c>
-      <c r="D380" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -7918,10 +7924,10 @@
         <v>538</v>
       </c>
       <c r="C381" t="s">
+        <v>790</v>
+      </c>
+      <c r="D381" t="s">
         <v>791</v>
-      </c>
-      <c r="D381" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -7929,10 +7935,10 @@
         <v>479</v>
       </c>
       <c r="C382" t="s">
+        <v>792</v>
+      </c>
+      <c r="D382" t="s">
         <v>793</v>
-      </c>
-      <c r="D382" t="s">
-        <v>794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>